<commit_message>
Add json parser and rename meta fields
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="calendar" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="event" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="category" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="lifecycle" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1140,7 +1140,7 @@
       <selection pane="topLeft" activeCell="Q57" activeCellId="0" sqref="Q57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
@@ -16785,8 +16785,8 @@
     <mergeCell ref="G139:G141"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="105" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="105" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -16801,14 +16801,14 @@
   </sheetPr>
   <dimension ref="A1:C1001"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="63.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="4" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
@@ -17897,8 +17897,8 @@
     <row r="1001" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -17913,11 +17913,11 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="10"/>
   </cols>
@@ -18959,8 +18959,8 @@
     <row r="1000" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>